<commit_message>
Revert "Merge branch 'main' of https://github.com/emilcarle/urban_sustainability_exam"
This reverts commit 625ede44e582dc10621e018b876d1910b3c23fa9, reversing
changes made to 6ec1718bdbf5d9cbf760e9332ac359ea4a8735b3.
</commit_message>
<xml_diff>
--- a/approach/index_allergenetic_trees.xlsx
+++ b/approach/index_allergenetic_trees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janisklug/Documents/HU_Berlin/Applied_Geoinformation_Science/Project_Work/urban_sustainability_exam/approach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8372E0BF-CE4D-2641-B6B9-662AA24743ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C479B-BCEE-4A44-AB4F-3037C8AB10D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3B7B1286-997D-FD41-8960-82FB8D0BF8C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3B7B1286-997D-FD41-8960-82FB8D0BF8C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -643,7 +643,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="88" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>